<commit_message>
first commit of the Altium project
</commit_message>
<xml_diff>
--- a/TP2/Calculos Flyback.xlsx
+++ b/TP2/Calculos Flyback.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico Bustelo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico Bustelo\Desktop\Electronics\0-GitHub\TPs-G1_E4\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61170C6-A6C3-4BEA-89C1-4D46B8920C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B4B51-C58C-4D90-B809-CA997D8A9BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Param</t>
   </si>
@@ -132,6 +132,15 @@
   </si>
   <si>
     <t>SI &gt;0 no entramos en modo disc</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>N3/N1</t>
+  </si>
+  <si>
+    <t>L3</t>
   </si>
 </sst>
 </file>
@@ -139,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -308,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -347,12 +356,6 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -366,14 +369,25 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -387,22 +401,6 @@
         <patternFill patternType="solid">
           <fgColor rgb="FF00FF00"/>
           <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -639,7 +637,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -696,7 +694,9 @@
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4">
+        <v>311</v>
+      </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -728,7 +728,9 @@
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4">
+        <v>16</v>
+      </c>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -819,7 +821,7 @@
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="20">
         <v>0.2</v>
       </c>
       <c r="C7" s="7"/>
@@ -851,7 +853,7 @@
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="19">
         <v>124</v>
       </c>
       <c r="C8" s="7"/>
@@ -883,13 +885,18 @@
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <f>B4/B3*(1/B7-1)</f>
         <v>6.4308681672025719E-2</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="25">
+        <f>E4/E3</f>
+        <v>5.1446945337620578E-2</v>
+      </c>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
@@ -921,8 +928,13 @@
         <v>7.9742765273311891</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="D10" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="4">
+        <f>B4/B3</f>
+        <v>1.607717041800643E-2</v>
+      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -949,7 +961,7 @@
       <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C11" s="7"/>
@@ -981,7 +993,7 @@
       <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="16">
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C12" s="7"/>
@@ -1013,7 +1025,7 @@
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
         <f>PI()*4*0.0000001</f>
         <v>1.2566370614359173E-6</v>
       </c>
@@ -1046,7 +1058,7 @@
       <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="16">
         <v>260</v>
       </c>
       <c r="C14" s="7"/>
@@ -1078,7 +1090,7 @@
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="16">
         <f>(1/(B13*B12))*(B11/B14+B5)</f>
         <v>6070332.7653639568</v>
       </c>
@@ -1111,7 +1123,7 @@
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <f>B10*B6/(B15*B12*(1-B7))</f>
         <v>0.10947061217729194</v>
       </c>
@@ -1144,7 +1156,7 @@
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="18">
+      <c r="B17" s="16">
         <f>0.5*B7/B20*B3/(B8*B12)</f>
         <v>2.7867383512544804E-2</v>
       </c>
@@ -1177,7 +1189,7 @@
       <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="16">
         <f>B16+B17</f>
         <v>0.13733799568983673</v>
       </c>
@@ -1212,7 +1224,7 @@
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="16">
         <v>0.2</v>
       </c>
       <c r="C19" s="7"/>
@@ -1244,14 +1256,19 @@
       <c r="A20" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="16">
         <v>150000</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="D20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="24">
+        <f>B21*E10</f>
+        <v>4.0723067729952597E-5</v>
+      </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
@@ -1278,13 +1295,18 @@
       <c r="A21" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="16">
         <f>B8^2/B15</f>
         <v>2.5329748128030518E-3</v>
       </c>
       <c r="C21" s="7"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="24">
+        <f>B21*E9</f>
+        <v>1.3031381673584832E-4</v>
+      </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -1311,7 +1333,7 @@
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="18">
+      <c r="B22" s="16">
         <f>B3*B7/B20/B21</f>
         <v>0.1637073786011265</v>
       </c>
@@ -1344,7 +1366,7 @@
       <c r="A23" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="21">
         <f>B24+B22/2</f>
         <v>0.40339709766069182</v>
       </c>
@@ -1377,7 +1399,7 @@
       <c r="A24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="21">
         <f>B6*B9/(1-B7)</f>
         <v>0.32154340836012857</v>
       </c>
@@ -1410,14 +1432,14 @@
       <c r="A25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="23">
+      <c r="B25" s="21">
         <f>B24-B23/2</f>
         <v>0.11984485952978266</v>
       </c>
-      <c r="C25" s="16" t="s">
+      <c r="C25" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="17"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1445,7 +1467,7 @@
       <c r="A26" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>2.8999999999999998E-7</v>
       </c>
       <c r="C26" s="7"/>
@@ -1477,7 +1499,7 @@
       <c r="A27" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <f>1/B15</f>
         <v>1.647356147764732E-7</v>
       </c>
@@ -1510,7 +1532,7 @@
       <c r="A28" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <f>66/SQRT(B20)</f>
         <v>0.17041126723312636</v>
       </c>
@@ -1520,7 +1542,7 @@
     </row>
     <row r="29" spans="1:26" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
-      <c r="B29" s="20"/>
+      <c r="B29" s="18"/>
     </row>
     <row r="30" spans="1:26" ht="18.600000000000001" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
@@ -1531,10 +1553,10 @@
     <mergeCell ref="C25:D25"/>
   </mergeCells>
   <conditionalFormatting sqref="B18">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0.2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update schematic & simulation (add ESR cap)
</commit_message>
<xml_diff>
--- a/TP2/Calculos Flyback.xlsx
+++ b/TP2/Calculos Flyback.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico Bustelo\Desktop\Electronics\0-GitHub\TPs-G1_E4\TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69B4B51-C58C-4D90-B809-CA997D8A9BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B2E1D8-7D68-4529-92F3-347FCFB479F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4020" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Param</t>
   </si>
@@ -141,14 +141,21 @@
   </si>
   <si>
     <t>L3</t>
+  </si>
+  <si>
+    <t>N1/N2</t>
+  </si>
+  <si>
+    <t>N3/N1 REAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -317,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -372,17 +379,20 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,7 +647,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -645,6 +655,8 @@
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
     <col min="2" max="2" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -790,7 +802,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="4"/>
@@ -885,7 +897,7 @@
       <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="24">
         <f>B4/B3*(1/B7-1)</f>
         <v>6.4308681672025719E-2</v>
       </c>
@@ -893,11 +905,14 @@
       <c r="D9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="27">
         <f>E4/E3</f>
         <v>5.1446945337620578E-2</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="4">
+        <f>1/E9</f>
+        <v>19.4375</v>
+      </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -928,15 +943,20 @@
         <v>7.9742765273311891</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="22" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4">
         <f>B4/B3</f>
         <v>1.607717041800643E-2</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="F10" s="4">
+        <f>1/E10</f>
+        <v>62.2</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -997,8 +1017,13 @@
         <v>6.0000000000000002E-5</v>
       </c>
       <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="4">
+        <f>E9*(1/B7-1)</f>
+        <v>0.20578778135048231</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
@@ -1125,7 +1150,7 @@
       </c>
       <c r="B16" s="16">
         <f>B10*B6/(B15*B12*(1-B7))</f>
-        <v>0.10947061217729194</v>
+        <v>8.2102959132968958E-2</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="4"/>
@@ -1191,7 +1216,7 @@
       </c>
       <c r="B18" s="16">
         <f>B16+B17</f>
-        <v>0.13733799568983673</v>
+        <v>0.10997034264551377</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>19</v>
@@ -1265,9 +1290,9 @@
       <c r="D20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="24">
-        <f>B21*E10</f>
-        <v>4.0723067729952597E-5</v>
+      <c r="E20" s="23">
+        <f>B21*(E10^2)</f>
+        <v>6.547116998384662E-7</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1303,9 +1328,9 @@
       <c r="D21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="24">
-        <f>B21*E9</f>
-        <v>1.3031381673584832E-4</v>
+      <c r="E21" s="23">
+        <f>B21*(E9^2)</f>
+        <v>6.7042478063458945E-6</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1368,7 +1393,7 @@
       </c>
       <c r="B23" s="21">
         <f>B24+B22/2</f>
-        <v>0.40339709766069182</v>
+        <v>0.32301124557065969</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="4"/>
@@ -1401,7 +1426,7 @@
       </c>
       <c r="B24" s="21">
         <f>B6*B9/(1-B7)</f>
-        <v>0.32154340836012857</v>
+        <v>0.24115755627009644</v>
       </c>
       <c r="C24" s="7"/>
       <c r="D24" s="4"/>
@@ -1434,12 +1459,12 @@
       </c>
       <c r="B25" s="21">
         <f>B24-B23/2</f>
-        <v>0.11984485952978266</v>
-      </c>
-      <c r="C25" s="22" t="s">
+        <v>7.9651933484766596E-2</v>
+      </c>
+      <c r="C25" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="26"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>

</xml_diff>